<commit_message>
Lesson 16 - Connect to local DB
</commit_message>
<xml_diff>
--- a/MongoDB-2022.xlsx
+++ b/MongoDB-2022.xlsx
@@ -5,18 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\OneDrive\Desktop\Mongo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\OneDrive\Desktop\Mongo\Alter-Bill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC52FDA0-AB27-4C0C-8D4D-38EC3F699558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46488D78-79D2-4882-8C05-13079E0BCADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
-    <sheet name="NodeJS Driver" sheetId="3" r:id="rId2"/>
-    <sheet name="app.js basics" sheetId="4" r:id="rId3"/>
-    <sheet name="Installing" sheetId="2" r:id="rId4"/>
+    <sheet name="db.js" sheetId="5" r:id="rId2"/>
+    <sheet name="NodeJS Driver" sheetId="3" r:id="rId3"/>
+    <sheet name="app.js basics" sheetId="4" r:id="rId4"/>
+    <sheet name="Installing" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t xml:space="preserve">Go To this page to download the local MongoDB </t>
   </si>
@@ -559,13 +561,706 @@
   </si>
   <si>
     <t>Build the basics of the app.js file</t>
+  </si>
+  <si>
+    <t>Create the db.js file to connect to the database</t>
+  </si>
+  <si>
+    <t>      })</t>
+  </si>
+  <si>
+    <t>  },</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <r>
+      <t>const</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> { </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MongoClient</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> } </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>require</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF98C379"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'mongodb'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>let</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>dbConnection</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>module</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>exports</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>connectToDb</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>cb</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MongoClient</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>connect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF98C379"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'mongodb://localhost:27017/bookstore'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>      .</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>client</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>dbConnection</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>client</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>db</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>return</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>cb</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>      .</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>catch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>err</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>console</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>log</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>err</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>return</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>cb</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>err</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>getDb</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: () </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>dbConnection</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -686,8 +1381,50 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC678DD"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFABB2BF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFE5C07B"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF56B6C2"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF61AFEF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF98C379"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFE06C75"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -712,6 +1449,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -726,16 +1469,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -783,6 +1520,25 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1066,35 +1822,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:A5"/>
+  <dimension ref="A2:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.1796875" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" style="11"/>
+    <col min="1" max="1" width="16.1796875" style="9"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="9" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A6" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1106,6 +1867,111 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BEFAE4-3CA8-4F7E-828E-3AFE3E35D56C}">
+  <dimension ref="A1:A18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="16384" width="8.7265625" style="25"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="26"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="26"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" s="28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" s="28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" s="28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" s="28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" s="28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF3B01D-16F6-42B7-86CB-E827FF47438A}">
   <dimension ref="A1:H8"/>
   <sheetViews>
@@ -1115,8 +1981,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="15"/>
-    <col min="2" max="16384" width="8.7265625" style="12"/>
+    <col min="1" max="1" width="8.7265625" style="13"/>
+    <col min="2" max="16384" width="8.7265625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1125,54 +1991,54 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-    </row>
-    <row r="4" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+    </row>
+    <row r="4" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="12">
         <v>1</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="15">
+      <c r="A5" s="13">
         <v>2</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14">
+    <row r="6" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="12">
         <v>3</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14">
+    <row r="7" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="12">
         <v>4</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14">
+    <row r="8" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="12">
         <v>5</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1185,7 +2051,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E3D431-AA03-4F95-9AC5-2142B721FC14}">
   <dimension ref="A1:H16"/>
   <sheetViews>
@@ -1195,7 +2061,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="16"/>
+    <col min="1" max="16384" width="8.7265625" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1203,69 +2069,69 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="18" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="18" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="19"/>
-    </row>
-    <row r="5" spans="1:8" s="18" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="20" t="s">
+    <row r="4" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="17"/>
+    </row>
+    <row r="5" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="18" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="18" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="19"/>
-    </row>
-    <row r="8" spans="1:8" s="18" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="21" t="s">
+    <row r="7" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="17"/>
+    </row>
+    <row r="8" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="18" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="22" t="s">
+    <row r="9" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="18" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="22" t="s">
+    <row r="10" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="18" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="19"/>
-    </row>
-    <row r="12" spans="1:8" s="18" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="20" t="s">
+    <row r="11" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="17"/>
+    </row>
+    <row r="12" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="18" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="21" t="s">
+    <row r="13" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="18" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="22" t="s">
+    <row r="14" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="18" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="22" t="s">
+    <row r="15" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="18" customFormat="1" ht="18.5" x14ac:dyDescent="0.45"/>
+    <row r="16" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="Home!A1" display="Home" xr:uid="{49D73059-F31D-4AB5-A97E-01B018A306B0}"/>
@@ -1274,7 +2140,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CAF8FD-270C-441E-BCAF-AAE71125610D}">
   <dimension ref="A1:N11"/>
   <sheetViews>
@@ -1282,10 +2148,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.453125" style="6" customWidth="1"/>
-    <col min="2" max="5" width="8.7265625" style="4"/>
-    <col min="6" max="6" width="8.7265625" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="10.453125" style="4" customWidth="1"/>
+    <col min="2" max="5" width="8.7265625" style="2"/>
+    <col min="6" max="6" width="8.7265625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
@@ -1294,85 +2160,85 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="3" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="8">
+      <c r="C6" s="22"/>
+    </row>
+    <row r="7" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
         <v>5</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="8"/>
-    </row>
-    <row r="9" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="7">
+    <row r="8" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6"/>
+    </row>
+    <row r="9" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="7"/>
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5"/>
+      <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="7"/>
+    <row r="11" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1389,4 +2255,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7AFA27-FA48-41B7-A4C4-E830A8C7AAC6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Lesson 17 - Fetching all docs
</commit_message>
<xml_diff>
--- a/MongoDB-2022.xlsx
+++ b/MongoDB-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\OneDrive\Desktop\Mongo\Alter-Bill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46488D78-79D2-4882-8C05-13079E0BCADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EC1FE8-955B-4BF7-BC50-ADB7E63EAE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="NodeJS Driver" sheetId="3" r:id="rId3"/>
     <sheet name="app.js basics" sheetId="4" r:id="rId4"/>
     <sheet name="Installing" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
+    <sheet name="Node&amp;Mongo functions" sheetId="6" r:id="rId6"/>
+    <sheet name="Fetch All docs" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t xml:space="preserve">Go To this page to download the local MongoDB </t>
   </si>
@@ -1253,6 +1254,385 @@
         <family val="3"/>
       </rPr>
       <t>dbConnection</t>
+    </r>
+  </si>
+  <si>
+    <t>db.collection('collectionName')</t>
+  </si>
+  <si>
+    <t>.find()</t>
+  </si>
+  <si>
+    <t>.find().sort({ date: 1})</t>
+  </si>
+  <si>
+    <t>.find().forEach(bill =&gt; myNewArray.push(bill) )</t>
+  </si>
+  <si>
+    <t>.then((results) =&gt; {
+   res.status(200).json(results)
+})</t>
+  </si>
+  <si>
+    <t>.catch(() =&gt; {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   res.status(500).json({ error: 'Could not succed'})</t>
+  </si>
+  <si>
+    <t>  })</t>
+  </si>
+  <si>
+    <r>
+      <t>app</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>get</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF98C379"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'/bills'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>, (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>req</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>db</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>collection</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF98C379"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'alter-bills'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>find</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>().</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>toArray</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>  .</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>((</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>results</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>500</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>json</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>results</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
     </r>
   </si>
 </sst>
@@ -1469,7 +1849,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1522,12 +1902,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1540,6 +1914,18 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1870,98 +2256,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BEFAE4-3CA8-4F7E-828E-3AFE3E35D56C}">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="25"/>
+    <col min="1" max="16384" width="8.7265625" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="26"/>
+      <c r="A2" s="24"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="22" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="26"/>
+      <c r="A4" s="24"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="25" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="26" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="26" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="26" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="26" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="26" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="26" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="26" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="26" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="26" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="26" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="26" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="26" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2163,54 +2549,54 @@
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="27"/>
     </row>
     <row r="7" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
@@ -2259,12 +2645,109 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7AFA27-FA48-41B7-A4C4-E830A8C7AAC6}">
-  <dimension ref="A1"/>
+  <dimension ref="A3:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="38.26953125" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.7265625" style="29"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" s="29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" s="29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C09B30-7F20-4B08-A7B4-0026A51D453B}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="16384" width="8.7265625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lesson 19 - Fetching Single Document
</commit_message>
<xml_diff>
--- a/MongoDB-2022.xlsx
+++ b/MongoDB-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\OneDrive\Desktop\Mongo\Alter-Bill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EC1FE8-955B-4BF7-BC50-ADB7E63EAE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9876EA4-5A9D-48DC-A673-595B75A658DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Installing" sheetId="2" r:id="rId5"/>
     <sheet name="Node&amp;Mongo functions" sheetId="6" r:id="rId6"/>
     <sheet name="Fetch All docs" sheetId="7" r:id="rId7"/>
+    <sheet name="Get Single Doc" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
   <si>
     <t xml:space="preserve">Go To this page to download the local MongoDB </t>
   </si>
@@ -1633,6 +1634,984 @@
         <family val="3"/>
       </rPr>
       <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Fetch All Documents</t>
+  </si>
+  <si>
+    <t>You have to add this line first</t>
+  </si>
+  <si>
+    <t>const { ObjectId } = require('mongodb')</t>
+  </si>
+  <si>
+    <t>.findOne({})</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t>  }</t>
+  </si>
+  <si>
+    <r>
+      <t>app</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>get</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF98C379"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'/bills/:id'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>, (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>req</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ObjectId</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>isValid</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>req</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>params</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>db</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>collection</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF98C379"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'alter-bills'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>      .</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>findOne</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>({</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>_id</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>new</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ObjectId</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>req</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>params</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)})</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>      .</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>doc</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>200</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>).</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>json</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>doc</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>      .</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>catch</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>err</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>500</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>).</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>json</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>({</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>error</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF98C379"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Could not fetch the document'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>})</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  } </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>else</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>500</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>).</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>json</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>({</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>error</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF98C379"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Could not fetch the document'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>})</t>
     </r>
   </si>
 </sst>
@@ -1640,7 +2619,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1803,8 +2782,78 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFE5C07B"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFABB2BF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF61AFEF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF98C379"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFE06C75"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFC678DD"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFD19A66"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1835,8 +2884,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1844,12 +2899,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1872,8 +2936,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1915,17 +2977,54 @@
     <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2208,47 +3307,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:A6"/>
+  <dimension ref="A2:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.1796875" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="16.1796875" defaultRowHeight="27.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" style="9"/>
+    <col min="1" max="1" width="16.1796875" style="29"/>
+    <col min="2" max="16384" width="16.1796875" style="30"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="32" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="33" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A6" s="9" t="s">
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+    </row>
+    <row r="6" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="33" t="s">
         <v>29</v>
       </c>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+    </row>
+    <row r="7" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="33"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:B7"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" location="Installing!A1" display="Installing!A1" xr:uid="{679BB0D5-3BA8-4A26-94E0-EE157AC5B186}"/>
+    <hyperlink ref="A4" location="'NodeJS Driver'!A1" display="NodeJS Driver" xr:uid="{45F31791-54FF-4C41-9628-37AFA935C6AF}"/>
+    <hyperlink ref="A5:C5" location="'app.js basics'!A1" display="Build the basics of the app.js file" xr:uid="{CB73F767-2A48-49C2-94E4-B432D500898E}"/>
+    <hyperlink ref="A6:D6" location="db.js!A1" display="Create the db.js file to connect to the database" xr:uid="{E4DC8E2F-D010-4FDD-8E39-E7B0AE155B0A}"/>
+    <hyperlink ref="A7:B7" location="'Fetch All docs'!A1" display="Fetch All Documents" xr:uid="{94D8B899-6E32-473B-84D5-C680F65528FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2262,92 +3383,92 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="23"/>
+    <col min="1" max="16384" width="8.7265625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="24"/>
+      <c r="A2" s="22"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="20" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="24"/>
+      <c r="A4" s="22"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="24" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="24" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="24" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="24" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="24" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="24" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="24" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="24" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="24" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="24" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="24" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="24" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2361,14 +3482,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF3B01D-16F6-42B7-86CB-E827FF47438A}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="13"/>
-    <col min="2" max="16384" width="8.7265625" style="10"/>
+    <col min="1" max="1" width="8.7265625" style="11"/>
+    <col min="2" max="16384" width="8.7265625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -2377,54 +3496,54 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-    </row>
-    <row r="4" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="12">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+    </row>
+    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="10">
         <v>1</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="13">
+      <c r="A5" s="11">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="12">
+    <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="10">
         <v>3</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="12">
+    <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="10">
         <v>4</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="12">
+    <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="10">
         <v>5</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2441,13 +3560,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E3D431-AA03-4F95-9AC5-2142B721FC14}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="14"/>
+    <col min="1" max="16384" width="8.7265625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -2455,69 +3572,69 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="17"/>
-    </row>
-    <row r="5" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="18" t="s">
+    <row r="4" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="15"/>
+    </row>
+    <row r="5" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="17"/>
-    </row>
-    <row r="8" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="19" t="s">
+    <row r="7" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="15"/>
+    </row>
+    <row r="8" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="17"/>
-    </row>
-    <row r="12" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="18" t="s">
+    <row r="11" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="15"/>
+    </row>
+    <row r="12" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="19" t="s">
+    <row r="13" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="20" t="s">
+    <row r="14" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="20" t="s">
+    <row r="15" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="16" customFormat="1" ht="18.5" x14ac:dyDescent="0.45"/>
+    <row r="16" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="Home!A1" display="Home" xr:uid="{49D73059-F31D-4AB5-A97E-01B018A306B0}"/>
@@ -2645,56 +3762,61 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7AFA27-FA48-41B7-A4C4-E830A8C7AAC6}">
-  <dimension ref="A3:A14"/>
+  <dimension ref="A3:A16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.26953125" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.7265625" style="29"/>
+    <col min="1" max="1" width="38.26953125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.7265625" style="25"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="25" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="25" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="25" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="25" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="26" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="25" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="25" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="25" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" s="25" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2705,49 +3827,243 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C09B30-7F20-4B08-A7B4-0026A51D453B}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="16"/>
+    <col min="1" max="16384" width="8.7265625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:10" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="17" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="20" t="s">
+      <c r="J2" s="34"/>
+    </row>
+    <row r="3" spans="1:10" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="20" t="s">
+    <row r="4" spans="1:10" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="20" t="s">
+    <row r="5" spans="1:10" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="20" t="s">
+    <row r="6" spans="1:10" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="20" t="s">
+    <row r="7" spans="1:10" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="18" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Home!A1" display="Home" xr:uid="{73638B80-0B01-4F0D-88E0-57FCCA1E9222}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79362038-8BF9-4D86-8296-AE465F558A87}">
+  <dimension ref="A3:G23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="35"/>
+    <col min="2" max="2" width="38.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="8"/>
+    <col min="4" max="4" width="47.90625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="35">
+        <v>1</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+    </row>
+    <row r="6" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="11"/>
+      <c r="B6" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+    </row>
+    <row r="7" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="11"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+    </row>
+    <row r="8" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="11"/>
+      <c r="B8" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+    </row>
+    <row r="9" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="11"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+    </row>
+    <row r="10" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="11"/>
+      <c r="B10" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+    </row>
+    <row r="11" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="11"/>
+      <c r="B11" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+    </row>
+    <row r="12" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="11"/>
+      <c r="B12" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+    </row>
+    <row r="13" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="11"/>
+      <c r="B13" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+    </row>
+    <row r="14" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="11"/>
+      <c r="B14" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+    </row>
+    <row r="15" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="11"/>
+      <c r="B15" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+    </row>
+    <row r="16" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="11"/>
+      <c r="B16" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+    </row>
+    <row r="17" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="11"/>
+      <c r="B17" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+    </row>
+    <row r="18" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="11"/>
+      <c r="B18" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+    </row>
+    <row r="19" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="11"/>
+      <c r="B19" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+    </row>
+    <row r="20" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="11"/>
+      <c r="B20" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+    </row>
+    <row r="21" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="11"/>
+      <c r="B21" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+    </row>
+    <row r="22" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="11"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+    </row>
+    <row r="23" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="11"/>
+      <c r="B23" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Lesson 20 - Post Request
</commit_message>
<xml_diff>
--- a/MongoDB-2022.xlsx
+++ b/MongoDB-2022.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\OneDrive\Desktop\Mongo\Alter-Bill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9876EA4-5A9D-48DC-A673-595B75A658DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05761D9-7A97-4FC5-9D9C-506A547EC66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="768" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
-    <sheet name="db.js" sheetId="5" r:id="rId2"/>
-    <sheet name="NodeJS Driver" sheetId="3" r:id="rId3"/>
-    <sheet name="app.js basics" sheetId="4" r:id="rId4"/>
-    <sheet name="Installing" sheetId="2" r:id="rId5"/>
-    <sheet name="Node&amp;Mongo functions" sheetId="6" r:id="rId6"/>
-    <sheet name="Fetch All docs" sheetId="7" r:id="rId7"/>
-    <sheet name="Get Single Doc" sheetId="8" r:id="rId8"/>
+    <sheet name="Post Request" sheetId="9" r:id="rId2"/>
+    <sheet name="db.js" sheetId="5" r:id="rId3"/>
+    <sheet name="NodeJS Driver" sheetId="3" r:id="rId4"/>
+    <sheet name="app.js basics" sheetId="4" r:id="rId5"/>
+    <sheet name="Installing" sheetId="2" r:id="rId6"/>
+    <sheet name="Node&amp;Mongo functions" sheetId="6" r:id="rId7"/>
+    <sheet name="Fetch All docs" sheetId="7" r:id="rId8"/>
+    <sheet name="Get Single Doc" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="86">
   <si>
     <t xml:space="preserve">Go To this page to download the local MongoDB </t>
   </si>
@@ -2606,6 +2607,637 @@
     <r>
       <rPr>
         <b/>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>})</t>
+    </r>
+  </si>
+  <si>
+    <t>Get Single Document</t>
+  </si>
+  <si>
+    <t>app.use(express.json())</t>
+  </si>
+  <si>
+    <t>to let express accepts the jsoned data that comes with post request</t>
+  </si>
+  <si>
+    <t>Post Request</t>
+  </si>
+  <si>
+    <t>    })</t>
+  </si>
+  <si>
+    <r>
+      <t>app</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>post</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF98C379"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'/books'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>, (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>req</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>const</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>req</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>body</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>db</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>collection</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF98C379"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'books'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    .</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>insertOne</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE5C07B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    .</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>result</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>201</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>json</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>result</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    .</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>catch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>err</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>500</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF61AFEF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>json</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>({</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>err</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF98C379"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Could not create new document'</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="12"/>
         <color rgb="FFABB2BF"/>
         <rFont val="Consolas"/>
@@ -2619,7 +3251,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="38" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2852,6 +3484,26 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="5"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFD19A66"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -2913,7 +3565,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2983,12 +3635,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3000,9 +3646,6 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3024,6 +3667,34 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3307,59 +3978,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.1796875" defaultRowHeight="27.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" style="29"/>
-    <col min="2" max="16384" width="16.1796875" style="30"/>
+    <col min="1" max="1" width="16.1796875" style="27"/>
+    <col min="2" max="16384" width="16.1796875" style="28"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="27" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="30" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
     </row>
     <row r="6" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
     </row>
     <row r="7" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="33"/>
+      <c r="B7" s="43"/>
+    </row>
+    <row r="8" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="43"/>
+    </row>
+    <row r="9" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="27" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" location="Installing!A1" display="Installing!A1" xr:uid="{679BB0D5-3BA8-4A26-94E0-EE157AC5B186}"/>
@@ -3367,6 +4050,7 @@
     <hyperlink ref="A5:C5" location="'app.js basics'!A1" display="Build the basics of the app.js file" xr:uid="{CB73F767-2A48-49C2-94E4-B432D500898E}"/>
     <hyperlink ref="A6:D6" location="db.js!A1" display="Create the db.js file to connect to the database" xr:uid="{E4DC8E2F-D010-4FDD-8E39-E7B0AE155B0A}"/>
     <hyperlink ref="A7:B7" location="'Fetch All docs'!A1" display="Fetch All Documents" xr:uid="{94D8B899-6E32-473B-84D5-C680F65528FA}"/>
+    <hyperlink ref="A8:B8" location="'Get Single Doc'!A1" display="Get Single Document" xr:uid="{AA4CD444-09D3-49E9-8B4F-33FB47645CDE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -3374,11 +4058,101 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA1C15D-0ECC-44A9-BF2A-49645410081E}">
+  <dimension ref="A1:A22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" s="12" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="50" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="51" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="52"/>
+    </row>
+    <row r="6" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="51" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="51" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="51" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="51" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="51" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="51" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="51" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="51" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35"/>
+    <row r="17" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35"/>
+    <row r="18" s="12" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="19" s="12" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="20" s="12" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="21" s="12" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="22" s="12" customFormat="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Home!A1" display="Home" xr:uid="{066787BA-BDEE-4731-8525-C412133EFB91}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BEFAE4-3CA8-4F7E-828E-3AFE3E35D56C}">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3386,78 +4160,81 @@
     <col min="1" max="16384" width="8.7265625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="22"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="22"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="24" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="24" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="24" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="24" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="24" t="s">
         <v>31</v>
       </c>
@@ -3473,12 +4250,15 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K1" location="Home!A1" display="Home" xr:uid="{9DDFEC03-EC8C-4455-99C7-AC35B32F74FF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF3B01D-16F6-42B7-86CB-E827FF47438A}">
   <dimension ref="A1:H8"/>
   <sheetViews>
@@ -3556,9 +4336,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E3D431-AA03-4F95-9AC5-2142B721FC14}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3586,56 +4366,77 @@
       </c>
     </row>
     <row r="6" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="46" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="15"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+    </row>
+    <row r="7" spans="1:8" s="14" customFormat="1" ht="20.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="48" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="8" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="15"/>
+    </row>
+    <row r="9" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="17" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="18" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A10" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="15"/>
-    </row>
     <row r="12" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15"/>
+    </row>
+    <row r="13" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="17" t="s">
+    <row r="14" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H14" s="14" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="18" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A15" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A16" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45"/>
+    <row r="17" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:G7"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Home!A1" display="Home" xr:uid="{49D73059-F31D-4AB5-A97E-01B018A306B0}"/>
   </hyperlinks>
@@ -3643,7 +4444,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CAF8FD-270C-441E-BCAF-AAE71125610D}">
   <dimension ref="A1:N11"/>
   <sheetViews>
@@ -3666,54 +4467,54 @@
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28" t="s">
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="27"/>
+      <c r="C6" s="44"/>
     </row>
     <row r="7" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
@@ -3760,7 +4561,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7AFA27-FA48-41B7-A4C4-E830A8C7AAC6}">
   <dimension ref="A3:A16"/>
   <sheetViews>
@@ -3825,13 +4626,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C09B30-7F20-4B08-A7B4-0026A51D453B}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
@@ -3847,7 +4646,7 @@
       <c r="A2" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="34"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="3" spans="1:10" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="18" t="s">
@@ -3883,187 +4682,193 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79362038-8BF9-4D86-8296-AE465F558A87}">
-  <dimension ref="A3:G23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="35"/>
+    <col min="1" max="1" width="8.7265625" style="32"/>
     <col min="2" max="2" width="38.26953125" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7265625" style="8"/>
     <col min="4" max="4" width="47.90625" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.7265625" style="8"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="35">
+      <c r="A3" s="32">
         <v>1</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="37"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-    </row>
-    <row r="6" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+    </row>
+    <row r="6" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11"/>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-    </row>
-    <row r="7" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+    </row>
+    <row r="7" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-    </row>
-    <row r="8" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="41"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+    </row>
+    <row r="8" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11"/>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-    </row>
-    <row r="9" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+    </row>
+    <row r="9" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-    </row>
-    <row r="10" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="41"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+    </row>
+    <row r="10" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11"/>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-    </row>
-    <row r="11" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+    </row>
+    <row r="11" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11"/>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-    </row>
-    <row r="12" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+    </row>
+    <row r="12" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11"/>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-    </row>
-    <row r="13" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+    </row>
+    <row r="13" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11"/>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-    </row>
-    <row r="14" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+    </row>
+    <row r="14" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11"/>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-    </row>
-    <row r="15" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+    </row>
+    <row r="15" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11"/>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-    </row>
-    <row r="16" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+    </row>
+    <row r="16" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11"/>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-    </row>
-    <row r="17" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+    </row>
+    <row r="17" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11"/>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-    </row>
-    <row r="18" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+    </row>
+    <row r="18" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11"/>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-    </row>
-    <row r="19" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+    </row>
+    <row r="19" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11"/>
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-    </row>
-    <row r="20" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+    </row>
+    <row r="20" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11"/>
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-    </row>
-    <row r="21" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+    </row>
+    <row r="21" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11"/>
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-    </row>
-    <row r="22" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+    </row>
+    <row r="22" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11"/>
-      <c r="B22" s="44"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-    </row>
-    <row r="23" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="41"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+    </row>
+    <row r="23" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="11"/>
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Home!A1" display="Home" xr:uid="{A11FB368-5EC9-4C1B-88AA-39F38D43A96F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lesson 21 - Delete Document
</commit_message>
<xml_diff>
--- a/MongoDB-2022.xlsx
+++ b/MongoDB-2022.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\OneDrive\Desktop\Mongo\Alter-Bill\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\total tech co\Desktop\Self-Study\MongoDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05761D9-7A97-4FC5-9D9C-506A547EC66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12895C3D-D1DE-446C-A260-0DFD5D9BA589}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="768" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="768" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
-    <sheet name="Post Request" sheetId="9" r:id="rId2"/>
-    <sheet name="db.js" sheetId="5" r:id="rId3"/>
-    <sheet name="NodeJS Driver" sheetId="3" r:id="rId4"/>
-    <sheet name="app.js basics" sheetId="4" r:id="rId5"/>
-    <sheet name="Installing" sheetId="2" r:id="rId6"/>
-    <sheet name="Node&amp;Mongo functions" sheetId="6" r:id="rId7"/>
-    <sheet name="Fetch All docs" sheetId="7" r:id="rId8"/>
-    <sheet name="Get Single Doc" sheetId="8" r:id="rId9"/>
+    <sheet name="Delete Doc" sheetId="10" r:id="rId2"/>
+    <sheet name="Post Request" sheetId="9" r:id="rId3"/>
+    <sheet name="db.js" sheetId="5" r:id="rId4"/>
+    <sheet name="NodeJS Driver" sheetId="3" r:id="rId5"/>
+    <sheet name="app.js basics" sheetId="4" r:id="rId6"/>
+    <sheet name="Installing" sheetId="2" r:id="rId7"/>
+    <sheet name="Node&amp;Mongo functions" sheetId="6" r:id="rId8"/>
+    <sheet name="Fetch All docs" sheetId="7" r:id="rId9"/>
+    <sheet name="Get Single Doc" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="107">
   <si>
     <t xml:space="preserve">Go To this page to download the local MongoDB </t>
   </si>
@@ -3240,6 +3241,1747 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>})</t>
+    </r>
+  </si>
+  <si>
+    <t>Delete Document</t>
+  </si>
+  <si>
+    <r>
+      <t>app</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>delete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'/bills/:id'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>, (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>req</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFC586C0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF4EC9B0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ObjectId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>isValid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>req</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>params</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>db</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>collection</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'alter-bills'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>      .</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>deleteOne</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>({</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>_id:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>new</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF4EC9B0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ObjectId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>req</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>params</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)})</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>      .</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>result</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>json</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>result</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>      .</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>catch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>err</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>500</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>json</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>({</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>error:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Could not delete the document'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>})</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  } </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFC586C0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>else</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>500</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>json</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>({</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>error:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Could not fetch the document'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>})</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>app</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>delete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'/bills/:id'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>, (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>req</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFC586C0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF4EC9B0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ObjectId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>isValid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>req</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>params</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>db</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>collection</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'alter-bills'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>      .</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>deleteOne</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>({</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>_id:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>new</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF4EC9B0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ObjectId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>req</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>params</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)})</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>      .</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>result</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>json</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>result</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>      .</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>catch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>err</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>500</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>json</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>({</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>error:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Could not delete the document'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>})</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  } </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFC586C0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>else</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>500</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>json</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>({</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>error:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Could not fetch the document'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFD4D4D4"/>
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
@@ -3251,7 +4993,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="49" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3504,8 +5246,77 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF4FC1FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFDCDCAA"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF9CDCFE"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF569CD6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFC586C0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF4EC9B0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3542,6 +5353,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -3565,7 +5382,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3669,21 +5486,6 @@
     <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3697,6 +5499,36 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3978,71 +5810,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D9"/>
+  <dimension ref="A2:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.1796875" defaultRowHeight="27.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="16.21875" defaultRowHeight="27.45" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" style="27"/>
-    <col min="2" max="16384" width="16.1796875" style="28"/>
+    <col min="1" max="1" width="16.21875" style="27"/>
+    <col min="2" max="16384" width="16.21875" style="28"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="27.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="27.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="27.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="43" t="s">
+    <row r="5" spans="1:4" ht="27.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-    </row>
-    <row r="6" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="43" t="s">
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+    </row>
+    <row r="6" spans="1:4" ht="27.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-    </row>
-    <row r="7" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="43" t="s">
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+    </row>
+    <row r="7" spans="1:4" ht="27.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="43"/>
-    </row>
-    <row r="8" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="43" t="s">
+      <c r="B7" s="48"/>
+    </row>
+    <row r="8" spans="1:4" ht="27.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="43"/>
-    </row>
-    <row r="9" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="48"/>
+    </row>
+    <row r="9" spans="1:4" ht="27.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
         <v>76</v>
       </c>
     </row>
+    <row r="10" spans="1:4" ht="27.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="48"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" location="Installing!A1" display="Installing!A1" xr:uid="{679BB0D5-3BA8-4A26-94E0-EE157AC5B186}"/>
@@ -4051,94 +5890,390 @@
     <hyperlink ref="A6:D6" location="db.js!A1" display="Create the db.js file to connect to the database" xr:uid="{E4DC8E2F-D010-4FDD-8E39-E7B0AE155B0A}"/>
     <hyperlink ref="A7:B7" location="'Fetch All docs'!A1" display="Fetch All Documents" xr:uid="{94D8B899-6E32-473B-84D5-C680F65528FA}"/>
     <hyperlink ref="A8:B8" location="'Get Single Doc'!A1" display="Get Single Document" xr:uid="{AA4CD444-09D3-49E9-8B4F-33FB47645CDE}"/>
+    <hyperlink ref="A10:B10" location="'Delete Doc'!A1" display="Delete Document" xr:uid="{B627612B-960F-4892-86BF-69C4740CBF95}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79362038-8BF9-4D86-8296-AE465F558A87}">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.77734375" style="32"/>
+    <col min="2" max="2" width="38.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" style="8"/>
+    <col min="4" max="4" width="47.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="32">
+        <v>1</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="34"/>
+      <c r="D3" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+    </row>
+    <row r="6" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+    </row>
+    <row r="7" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+    </row>
+    <row r="8" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+    </row>
+    <row r="9" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+    </row>
+    <row r="10" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+    </row>
+    <row r="11" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+      <c r="B11" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+    </row>
+    <row r="12" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="B12" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+    </row>
+    <row r="13" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+    </row>
+    <row r="14" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+    </row>
+    <row r="15" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
+      <c r="B15" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+    </row>
+    <row r="16" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+    </row>
+    <row r="17" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+    </row>
+    <row r="18" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+    </row>
+    <row r="19" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+    </row>
+    <row r="20" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+    </row>
+    <row r="21" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+    </row>
+    <row r="22" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+    </row>
+    <row r="23" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
+      <c r="B23" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Home!A1" display="Home" xr:uid="{A11FB368-5EC9-4C1B-88AA-39F38D43A96F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FB5D86-C542-4B5D-801A-6D00E4065D7C}">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="53"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:1" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="55" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="56" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="57"/>
+    </row>
+    <row r="6" spans="1:1" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="56" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="56" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="56" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="56" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="56" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="56" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A12" s="56" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" s="56" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A14" s="56" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="56" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="56" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A17" s="56" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A18" s="56" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Home!A1" display="Home" xr:uid="{4BE7D26D-8405-4D54-B75D-EC528F09EE77}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA1C15D-0ECC-44A9-BF2A-49645410081E}">
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" s="12" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" s="12" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="50" t="s">
+    <row r="2" spans="1:1" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:1" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="45" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="51" t="s">
+    <row r="4" spans="1:1" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="46" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="52"/>
-    </row>
-    <row r="6" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="51" t="s">
+    <row r="5" spans="1:1" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="47"/>
+    </row>
+    <row r="6" spans="1:1" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="46" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="51" t="s">
+    <row r="7" spans="1:1" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="46" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="51" t="s">
+    <row r="8" spans="1:1" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="46" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="51" t="s">
+    <row r="9" spans="1:1" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="46" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="51" t="s">
+    <row r="10" spans="1:1" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="46" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="51" t="s">
+    <row r="11" spans="1:1" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="46" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="51" t="s">
+    <row r="12" spans="1:1" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="46" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="51" t="s">
+    <row r="13" spans="1:1" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="46" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="51" t="s">
+    <row r="14" spans="1:1" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="46" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:1" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35"/>
-    <row r="17" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35"/>
-    <row r="18" s="12" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="19" s="12" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="20" s="12" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="21" s="12" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="22" s="12" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:1" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:1" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="17" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="18" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="Home!A1" display="Home" xr:uid="{066787BA-BDEE-4731-8525-C412133EFB91}"/>
@@ -4147,7 +6282,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BEFAE4-3CA8-4F7E-828E-3AFE3E35D56C}">
   <dimension ref="A1:K18"/>
   <sheetViews>
@@ -4155,12 +6290,12 @@
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="21"/>
+    <col min="1" max="16384" width="8.77734375" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>33</v>
       </c>
@@ -4168,83 +6303,83 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="22"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="22"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="s">
         <v>32</v>
       </c>
@@ -4258,24 +6393,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF3B01D-16F6-42B7-86CB-E827FF47438A}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="11"/>
-    <col min="2" max="16384" width="8.7265625" style="8"/>
+    <col min="1" max="1" width="8.77734375" style="11"/>
+    <col min="2" max="16384" width="8.77734375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>27</v>
       </c>
@@ -4287,7 +6422,7 @@
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
     </row>
-    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>1</v>
       </c>
@@ -4295,7 +6430,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>2</v>
       </c>
@@ -4303,7 +6438,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>3</v>
       </c>
@@ -4311,7 +6446,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>4</v>
       </c>
@@ -4319,7 +6454,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>5</v>
       </c>
@@ -4336,84 +6471,84 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E3D431-AA03-4F95-9AC5-2142B721FC14}">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="12"/>
+    <col min="1" max="16384" width="8.77734375" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="15"/>
     </row>
-    <row r="5" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="46" t="s">
+    <row r="6" spans="1:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-    </row>
-    <row r="7" spans="1:8" s="14" customFormat="1" ht="20.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="47" t="s">
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+    </row>
+    <row r="7" spans="1:8" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="48" t="s">
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="43" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="15"/>
     </row>
-    <row r="9" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="15"/>
     </row>
-    <row r="13" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
         <v>23</v>
       </c>
@@ -4421,17 +6556,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" s="14" customFormat="1" ht="18.5" x14ac:dyDescent="0.45"/>
+    <row r="17" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A6:D6"/>
@@ -4444,79 +6579,79 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CAF8FD-270C-441E-BCAF-AAE71125610D}">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.453125" style="4" customWidth="1"/>
-    <col min="2" max="5" width="8.7265625" style="2"/>
-    <col min="6" max="6" width="8.7265625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="10.44140625" style="4" customWidth="1"/>
+    <col min="2" max="5" width="8.77734375" style="2"/>
+    <col min="6" max="6" width="8.77734375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="45" t="s">
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="44"/>
-    </row>
-    <row r="7" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="51"/>
+    </row>
+    <row r="7" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -4524,10 +6659,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
     </row>
-    <row r="9" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>6</v>
       </c>
@@ -4535,13 +6670,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
     </row>
   </sheetData>
@@ -4561,7 +6696,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7AFA27-FA48-41B7-A4C4-E830A8C7AAC6}">
   <dimension ref="A3:A16"/>
   <sheetViews>
@@ -4569,53 +6704,53 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.26953125" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.7265625" style="25"/>
+    <col min="1" max="1" width="38.21875" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.77734375" style="25"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" ht="65.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
         <v>60</v>
       </c>
@@ -4626,49 +6761,49 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C09B30-7F20-4B08-A7B4-0026A51D453B}">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="24.45" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="14"/>
+    <col min="1" max="16384" width="8.77734375" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>53</v>
       </c>
       <c r="J2" s="31"/>
     </row>
-    <row r="3" spans="1:10" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18" t="s">
         <v>17</v>
       </c>
@@ -4680,195 +6815,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79362038-8BF9-4D86-8296-AE465F558A87}">
-  <dimension ref="A1:G23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="8.7265625" style="32"/>
-    <col min="2" max="2" width="38.26953125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="8"/>
-    <col min="4" max="4" width="47.90625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="32">
-        <v>1</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-    </row>
-    <row r="6" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="11"/>
-      <c r="B6" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-    </row>
-    <row r="7" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="11"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-    </row>
-    <row r="8" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="11"/>
-      <c r="B8" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-    </row>
-    <row r="9" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="11"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-    </row>
-    <row r="10" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="11"/>
-      <c r="B10" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-    </row>
-    <row r="11" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="11"/>
-      <c r="B11" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-    </row>
-    <row r="12" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="11"/>
-      <c r="B12" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-    </row>
-    <row r="13" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11"/>
-      <c r="B13" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-    </row>
-    <row r="14" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="11"/>
-      <c r="B14" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-    </row>
-    <row r="15" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11"/>
-      <c r="B15" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-    </row>
-    <row r="16" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="11"/>
-      <c r="B16" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-    </row>
-    <row r="17" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="11"/>
-      <c r="B17" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-    </row>
-    <row r="18" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="11"/>
-      <c r="B18" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-    </row>
-    <row r="19" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="11"/>
-      <c r="B19" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-    </row>
-    <row r="20" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="11"/>
-      <c r="B20" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-    </row>
-    <row r="21" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="11"/>
-      <c r="B21" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-    </row>
-    <row r="22" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="11"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-    </row>
-    <row r="23" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="11"/>
-      <c r="B23" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" location="Home!A1" display="Home" xr:uid="{A11FB368-5EC9-4C1B-88AA-39F38D43A96F}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>